<commit_message>
Add True False Test for Product
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/TestData/CMPG323 EcoPower Logistics Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/TestData/CMPG323 EcoPower Logistics Data.xlsx
@@ -2073,6 +2073,9 @@
       <x:c r="D2" s="0" t="n">
         <x:v>950</x:v>
       </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A3" s="0" t="n">
@@ -2086,6 +2089,9 @@
       </x:c>
       <x:c r="D3" s="0" t="n">
         <x:v>61</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix Order Details UI selection
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/TestData/CMPG323 EcoPower Logistics Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/TestData/CMPG323 EcoPower Logistics Data.xlsx
@@ -1108,6 +1108,9 @@
       <x:c r="E2" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A3" s="0" t="n">
@@ -1125,6 +1128,9 @@
       <x:c r="E3" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A4" s="0" t="n">
@@ -1142,6 +1148,9 @@
       <x:c r="E4" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A5" s="0" t="n">
@@ -1159,6 +1168,9 @@
       <x:c r="E5" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A6" s="0" t="n">
@@ -1176,6 +1188,9 @@
       <x:c r="E6" s="0" t="n">
         <x:v>0.7</x:v>
       </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A7" s="0" t="n">
@@ -1193,6 +1208,9 @@
       <x:c r="E7" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A8" s="0" t="n">
@@ -1210,6 +1228,9 @@
       <x:c r="E8" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A9" s="0" t="n">
@@ -1227,6 +1248,9 @@
       <x:c r="E9" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A10" s="0" t="n">
@@ -1244,6 +1268,9 @@
       <x:c r="E10" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A11" s="0" t="n">
@@ -1261,6 +1288,9 @@
       <x:c r="E11" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A12" s="0" t="n">
@@ -1278,6 +1308,9 @@
       <x:c r="E12" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A13" s="0" t="n">
@@ -1295,6 +1328,9 @@
       <x:c r="E13" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A14" s="0" t="n">
@@ -1312,6 +1348,9 @@
       <x:c r="E14" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A15" s="0" t="n">
@@ -1329,6 +1368,9 @@
       <x:c r="E15" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A16" s="0" t="n">
@@ -1346,6 +1388,9 @@
       <x:c r="E16" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A17" s="0" t="n">
@@ -1363,6 +1408,9 @@
       <x:c r="E17" s="0" t="n">
         <x:v>0.1</x:v>
       </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A18" s="0" t="n">
@@ -1380,6 +1428,9 @@
       <x:c r="E18" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A19" s="0" t="n">
@@ -1397,6 +1448,9 @@
       <x:c r="E19" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A20" s="0" t="n">
@@ -1414,6 +1468,9 @@
       <x:c r="E20" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A21" s="0" t="n">
@@ -1431,6 +1488,9 @@
       <x:c r="E21" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A22" s="0" t="n">
@@ -1448,6 +1508,9 @@
       <x:c r="E22" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A23" s="0" t="n">
@@ -1465,6 +1528,9 @@
       <x:c r="E23" s="0" t="n">
         <x:v>0.1</x:v>
       </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A24" s="0" t="n">
@@ -1482,6 +1548,9 @@
       <x:c r="E24" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F24" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A25" s="0" t="n">
@@ -1499,6 +1568,9 @@
       <x:c r="E25" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F25" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A26" s="0" t="n">
@@ -1516,6 +1588,9 @@
       <x:c r="E26" s="0" t="n">
         <x:v>0.1</x:v>
       </x:c>
+      <x:c r="F26" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A27" s="0" t="n">
@@ -1533,6 +1608,9 @@
       <x:c r="E27" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A28" s="0" t="n">
@@ -1550,6 +1628,9 @@
       <x:c r="E28" s="0" t="n">
         <x:v>0.1</x:v>
       </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A29" s="0" t="n">
@@ -1567,6 +1648,9 @@
       <x:c r="E29" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A30" s="0" t="n">
@@ -1584,6 +1668,9 @@
       <x:c r="E30" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F30" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A31" s="0" t="n">
@@ -1601,6 +1688,9 @@
       <x:c r="E31" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F31" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A32" s="0" t="n">
@@ -1618,6 +1708,9 @@
       <x:c r="E32" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F32" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A33" s="0" t="n">
@@ -1635,6 +1728,9 @@
       <x:c r="E33" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F33" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A34" s="0" t="n">
@@ -1652,6 +1748,9 @@
       <x:c r="E34" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F34" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A35" s="0" t="n">
@@ -1669,6 +1768,9 @@
       <x:c r="E35" s="0" t="n">
         <x:v>0.15</x:v>
       </x:c>
+      <x:c r="F35" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A36" s="0" t="n">
@@ -1686,6 +1788,9 @@
       <x:c r="E36" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F36" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A37" s="0" t="n">
@@ -1703,6 +1808,9 @@
       <x:c r="E37" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F37" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A38" s="0" t="n">
@@ -1720,6 +1828,9 @@
       <x:c r="E38" s="0" t="n">
         <x:v>0.2</x:v>
       </x:c>
+      <x:c r="F38" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A39" s="0" t="n">
@@ -1737,6 +1848,9 @@
       <x:c r="E39" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F39" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A40" s="0" t="n">
@@ -1754,6 +1868,9 @@
       <x:c r="E40" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="F40" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
     <x:row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A41" s="0" t="n">
@@ -1770,6 +1887,9 @@
       </x:c>
       <x:c r="E41" s="0" t="n">
         <x:v>0</x:v>
+      </x:c>
+      <x:c r="F41" s="0" t="s">
+        <x:v>9</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>